<commit_message>
fix docs. Add new behavior. if conv is NULL use the conv from @pp::sheet
2006-05-31  Jody Goldberg <jody@gnome.org>

	* src/parser.y (gnm_expr_parse_str) : fix docs.  Add new behavior.
	  if conv is NULL use the conv from @pp::sheet

	* src/parse-util.c (parse_text_value_or_expr) : Use the current
	  ExprConv associated with the ParsePosition's sheet, not
	  gnumeric_default (fixes R1C1).
	(gnm_expr_parse_str_simple) : ditto.
	* src/ranges.c (global_range_list_parse) : ditto.
	* src/value.c (value_new_cellrange_str) : ditto.
	* src/workbook-edit.c (wbcg_edit_finish) : ditto.
	* src/widgets/gnumeric-expr-entry.c (gnm_expr_entry_parse) : ditto.
</commit_message>
<xml_diff>
--- a/samples/excel12/cellstyle.xlsx
+++ b/samples/excel12/cellstyle.xlsx
@@ -1,60 +1,60 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.microsoft.com/office/excel/2006/2" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xml:space="preserve">
-  <fileVersion lastEdited="4" lowestEdited="4" rupBuild="3820"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/5/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion lastEdited="4" lowestEdited="4" rupBuild="4017"/>
   <workbookPr showInkAnnotation="0"/>
-  <calcPr calcId="122211" fullCalcOnLoad="1"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="120" windowWidth="19050" windowHeight="12195"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <calcPr calcId="122211"/>
   <webPublishing codePage="1252"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.microsoft.com/office/excel/2006/2" xml:space="preserve" count="81" uniqueCount="48">
-  <sstItem>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/5/main" count="81" uniqueCount="48">
+  <si>
     <t>CELL STYLES TEST SHEET</t>
-  </sstItem>
-  <sstItem>
+  </si>
+  <si>
     <t>Arioso</t>
-  </sstItem>
-  <sstItem>
+  </si>
+  <si>
     <t>text</t>
-  </sstItem>
-  <sstItem>
+  </si>
+  <si>
     <t>"Comma"</t>
-  </sstItem>
-  <sstItem>
+  </si>
+  <si>
     <t>"Currency"</t>
-  </sstItem>
-  <sstItem>
+  </si>
+  <si>
     <t>BUILT-IN STYLES</t>
-  </sstItem>
-  <sstItem>
+  </si>
+  <si>
     <t>"Percent"</t>
-  </sstItem>
-  <sstItem>
+  </si>
+  <si>
     <t>"Comma [0]"</t>
-  </sstItem>
-  <sstItem>
+  </si>
+  <si>
     <t>"Currency [0]"</t>
-  </sstItem>
-  <sstItem>
+  </si>
+  <si>
     <t>"RowLevel_1"</t>
-  </sstItem>
-  <sstItem>
+  </si>
+  <si>
     <t>"RowLevel_2"</t>
-  </sstItem>
-  <sstItem>
+  </si>
+  <si>
     <t>COND. FORMATTING</t>
-  </sstItem>
-  <sstItem>
-    <r>
-      <t>"Excel_BuiltIn_RowLevel_2" - must be </t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">"Excel_BuiltIn_RowLevel_2" - must be </t>
     </r>
     <r>
       <rPr>
@@ -66,10 +66,10 @@
       </rPr>
       <t>green</t>
     </r>
-  </sstItem>
-  <sstItem>
-    <r>
-      <t>"Excel_CondFormat_1_1" - must be </t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">"Excel_CondFormat_1_1" - must be </t>
     </r>
     <r>
       <rPr>
@@ -81,10 +81,10 @@
       </rPr>
       <t>blue</t>
     </r>
-  </sstItem>
-  <sstItem>
-    <r>
-      <t>"Standard" - must be </t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">"Standard" - must be </t>
     </r>
     <r>
       <rPr>
@@ -96,10 +96,10 @@
       </rPr>
       <t>purple</t>
     </r>
-  </sstItem>
-  <sstItem>
-    <r>
-      <t>"Result" - must be </t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">"Result" - must be </t>
     </r>
     <r>
       <rPr>
@@ -111,10 +111,10 @@
       </rPr>
       <t>dark green</t>
     </r>
-  </sstItem>
-  <sstItem>
-    <r>
-      <t>"Ergebnis" - must be </t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">"Ergebnis" - must be </t>
     </r>
     <r>
       <rPr>
@@ -126,10 +126,10 @@
       </rPr>
       <t>dark green</t>
     </r>
-  </sstItem>
-  <sstItem>
-    <r>
-      <t>"Default" - must be </t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">"Default" - must be </t>
     </r>
     <r>
       <rPr>
@@ -141,46 +141,46 @@
       </rPr>
       <t>purple</t>
     </r>
-  </sstItem>
-  <sstItem>
+  </si>
+  <si>
     <t>red</t>
-  </sstItem>
-  <sstItem>
+  </si>
+  <si>
     <t>yellow</t>
-  </sstItem>
-  <sstItem>
+  </si>
+  <si>
     <t>green</t>
-  </sstItem>
-  <sstItem>
+  </si>
+  <si>
     <t>no format</t>
-  </sstItem>
-  <sstItem>
+  </si>
+  <si>
     <t>Entire column Arioso/10pt - style "column-text" →</t>
-  </sstItem>
-  <sstItem>
+  </si>
+  <si>
     <t>← Arioso/14pt</t>
-  </sstItem>
-  <sstItem>
+  </si>
+  <si>
     <t>← black &amp; border</t>
-  </sstItem>
-  <sstItem>
+  </si>
+  <si>
     <t>← No style</t>
-  </sstItem>
-  <sstItem>
+  </si>
+  <si>
     <t>Row default overrides column default ↘</t>
-  </sstItem>
-  <sstItem>
+  </si>
+  <si>
     <t>Column default overrides row default ↘</t>
-  </sstItem>
-  <sstItem>
+  </si>
+  <si>
     <t>← Cell is aligned right/top &amp; rotated - style "align"</t>
-  </sstItem>
-  <sstItem>
+  </si>
+  <si>
     <t>← Cell has style "align" - with hard formatted 0°</t>
-  </sstItem>
-  <sstItem>
-    <r>
-      <t>"Excel_CondFormat_1_1_1" - must be </t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">"Excel_CondFormat_1_1_1" - must be </t>
     </r>
     <r>
       <rPr>
@@ -192,19 +192,19 @@
       </rPr>
       <t>yellow</t>
     </r>
-  </sstItem>
-  <sstItem>
+  </si>
+  <si>
     <t>← green &amp; border</t>
-  </sstItem>
-  <sstItem>
+  </si>
+  <si>
     <t>middle cell yellow ↘</t>
-  </sstItem>
-  <sstItem>
+  </si>
+  <si>
     <t>↙ Border only style - "border" ↘</t>
-  </sstItem>
-  <sstItem>
-    <r>
-      <t>↙ Entire column is </t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">↙ Entire column is </t>
     </r>
     <r>
       <rPr>
@@ -223,12 +223,12 @@
         <rFont val="Batang"/>
         <family val="1"/>
       </rPr>
-      <t> - style "column"</t>
-    </r>
-  </sstItem>
-  <sstItem>
-    <r>
-      <t>Entire column is </t>
+      <t xml:space="preserve"> - style "column"</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Entire column is </t>
     </r>
     <r>
       <rPr>
@@ -247,12 +247,12 @@
         <rFont val="Batang"/>
         <family val="1"/>
       </rPr>
-      <t> - hard format ↘</t>
-    </r>
-  </sstItem>
-  <sstItem>
-    <r>
-      <t>← Cell is </t>
+      <t xml:space="preserve"> - hard format ↘</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">← Cell is </t>
     </r>
     <r>
       <rPr>
@@ -271,12 +271,12 @@
         <rFont val="Batang"/>
         <family val="1"/>
       </rPr>
-      <t> - style "green", with hard-format borders</t>
-    </r>
-  </sstItem>
-  <sstItem>
-    <r>
-      <t>← Cell is </t>
+      <t xml:space="preserve"> - style "green", with hard-format borders</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">← Cell is </t>
     </r>
     <r>
       <rPr>
@@ -295,12 +295,12 @@
         <rFont val="Batang"/>
         <family val="1"/>
       </rPr>
-      <t> - cell style "green"</t>
-    </r>
-  </sstItem>
-  <sstItem>
-    <r>
-      <t>← Cell is </t>
+      <t xml:space="preserve"> - cell style "green"</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">← Cell is </t>
     </r>
     <r>
       <rPr>
@@ -319,12 +319,12 @@
         <rFont val="Batang"/>
         <family val="1"/>
       </rPr>
-      <t> - hard format</t>
-    </r>
-  </sstItem>
-  <sstItem>
-    <r>
-      <t>Entire sheet must be </t>
+      <t xml:space="preserve"> - hard format</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Entire sheet must be </t>
     </r>
     <r>
       <rPr>
@@ -343,12 +343,12 @@
         <rFont val="Batang"/>
         <family val="1"/>
       </rPr>
-      <t> and Batang/10pt</t>
-    </r>
-  </sstItem>
-  <sstItem>
-    <r>
-      <t>← Column default overridden with </t>
+      <t xml:space="preserve"> and Batang/10pt</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">← Column default overridden with </t>
     </r>
     <r>
       <rPr>
@@ -366,12 +366,12 @@
         <rFont val="Batang"/>
         <family val="1"/>
       </rPr>
-      <t> →</t>
-    </r>
-  </sstItem>
-  <sstItem>
-    <r>
-      <t>← Column default overridden with </t>
+      <t xml:space="preserve"> →</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">← Column default overridden with </t>
     </r>
     <r>
       <rPr>
@@ -390,12 +390,12 @@
         <rFont val="Batang"/>
         <family val="1"/>
       </rPr>
-      <t> →</t>
-    </r>
-  </sstItem>
-  <sstItem>
-    <r>
-      <t>↓ Row default overridden with </t>
+      <t xml:space="preserve"> →</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">↓ Row default overridden with </t>
     </r>
     <r>
       <rPr>
@@ -407,10 +407,10 @@
       </rPr>
       <t>red</t>
     </r>
-  </sstItem>
-  <sstItem>
-    <r>
-      <t>↓ Row default overridden with </t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">↓ Row default overridden with </t>
     </r>
     <r>
       <rPr>
@@ -421,10 +421,10 @@
       </rPr>
       <t>transp</t>
     </r>
-  </sstItem>
-  <sstItem>
-    <r>
-      <t>↓ Entire row is </t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">↓ Entire row is </t>
     </r>
     <r>
       <rPr>
@@ -443,12 +443,12 @@
         <rFont val="Batang"/>
         <family val="1"/>
       </rPr>
-      <t> - style "row"</t>
-    </r>
-  </sstItem>
-  <sstItem>
-    <r>
-      <t>↓ Entire row is </t>
+      <t xml:space="preserve"> - style "row"</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">↓ Entire row is </t>
     </r>
     <r>
       <rPr>
@@ -467,12 +467,12 @@
         <rFont val="Batang"/>
         <family val="1"/>
       </rPr>
-      <t> - hard format</t>
-    </r>
-  </sstItem>
-  <sstItem>
-    <r>
-      <t>"Hyperlink" - text must be </t>
+      <t xml:space="preserve"> - hard format</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">"Hyperlink" - text must be </t>
     </r>
     <r>
       <rPr>
@@ -485,15 +485,15 @@
       </rPr>
       <t>blue and underlined</t>
     </r>
-  </sstItem>
-  <sstItem>
+  </si>
+  <si>
     <t>Hyperlink</t>
-  </sstItem>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.microsoft.com/office/excel/2006/2" xml:space="preserve">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/5/main">
   <numFmts count="8">
     <numFmt numFmtId="164" formatCode="#,##0\ &quot;€&quot;;\-#,##0\ &quot;€&quot;"/>
     <numFmt numFmtId="165" formatCode="#,##0\ &quot;€&quot;;[Red]\-#,##0\ &quot;€&quot;"/>
@@ -932,23 +932,8 @@
       </fill>
     </dxf>
   </dxfs>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotTableStyle1"/>
-  <colors>
-    <themeColors>
-      <rgbColor rgb="FFFFFFFF"/>
-      <rgbColor rgb="FF000000"/>
-      <rgbColor rgb="FFEEECE1"/>
-      <rgbColor rgb="FF1F497D"/>
-      <rgbColor rgb="FF4F81BD"/>
-      <rgbColor rgb="FFC0504D"/>
-      <rgbColor rgb="FF9BBB59"/>
-      <rgbColor rgb="FF8064A2"/>
-      <rgbColor rgb="FF4BACC6"/>
-      <rgbColor rgb="FFF79646"/>
-      <rgbColor rgb="FF0000FF"/>
-      <rgbColor rgb="FF800080"/>
-    </themeColors>
-  </colors>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9"/>
+  <colors/>
 </styleSheet>
 </file>
 
@@ -1250,8 +1235,8 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.microsoft.com/office/excel/2006/2" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xml:space="preserve">
-  <sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/5/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr enableFormatConditionsCalculation="0">
     <outlinePr summaryBelow="0"/>
   </sheetPr>
   <dimension ref="A1:Q44"/>
@@ -1764,7 +1749,6 @@
       <c r="F44" s="59"/>
     </row>
   </sheetData>
-  <sheetProtection objects="0" scenarios="0"/>
   <phoneticPr fontId="0" type="noConversion"/>
   <conditionalFormatting sqref="D29:D32">
     <cfRule type="cellIs" dxfId="2" priority="2" stopIfTrue="1" operator="equal">

</xml_diff>